<commit_message>
AI update and added a parameter to RadialSpots analysis
</commit_message>
<xml_diff>
--- a/result_table_templates/RadialSpots_VC.xlsx
+++ b/result_table_templates/RadialSpots_VC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregschwartz/matlab/DJ_schwartzlab/result_table_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80776E90-906D-F84E-93BD-C59BDC1385E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF479E7-1742-0848-9C87-5EFF25EEE52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="960" windowWidth="46900" windowHeight="26720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7880" yWindow="1860" windowWidth="46900" windowHeight="26720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Field</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>peak inward current (pA) of traces in the same matrix format as trace_matrix_mean</t>
+  </si>
+  <si>
+    <t>charge_matrix</t>
+  </si>
+  <si>
+    <t>charge of each trace in trace_matrix_mean</t>
   </si>
 </sst>
 </file>
@@ -496,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="297" zoomScaleNormal="297" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -621,78 +627,89 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>28</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>